<commit_message>
okay, really need to clarify
</commit_message>
<xml_diff>
--- a/data/bdFile.xlsx
+++ b/data/bdFile.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lesleycheung/Desktop/mazen/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14A511D1-FBB8-724E-8CED-0AD10D801BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97613AF0-5467-A94E-B2BF-5448FAA86464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="3700" windowWidth="26840" windowHeight="15940" xr2:uid="{F2FF1488-102E-7448-BBB7-46247D1761A1}"/>
+    <workbookView xWindow="34800" yWindow="-21100" windowWidth="19200" windowHeight="21100" xr2:uid="{F2FF1488-102E-7448-BBB7-46247D1761A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$33</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -199,13 +202,27 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,15 +537,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F11435F-E248-4A4A-95C5-DA56F5DB2DC5}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F33"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -548,7 +572,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -566,7 +590,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
@@ -584,7 +608,7 @@
         <v>15.97</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -602,7 +626,7 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
@@ -638,7 +662,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -656,7 +680,7 @@
         <v>6.05</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -674,7 +698,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
@@ -694,7 +718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>22</v>
       </c>
@@ -714,7 +738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
@@ -734,7 +758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>45026</v>
       </c>
@@ -754,7 +778,7 @@
         <v>5.84</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>45026</v>
       </c>
@@ -772,7 +796,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>45148</v>
       </c>
@@ -790,7 +814,7 @@
         <v>1.62</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>45148</v>
       </c>
@@ -808,7 +832,7 @@
         <v>1.62</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>25</v>
       </c>
@@ -826,7 +850,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>25</v>
       </c>
@@ -844,7 +868,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -864,7 +888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>45026</v>
       </c>
@@ -884,7 +908,7 @@
         <v>58.8</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>45148</v>
       </c>
@@ -902,7 +926,7 @@
         <v>12.14</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -916,7 +940,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -934,7 +958,7 @@
         <v>2.4900000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -952,7 +976,7 @@
         <v>3.09</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>45026</v>
       </c>
@@ -970,7 +994,7 @@
         <v>37.35</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -988,7 +1012,7 @@
         <v>36.31</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -1006,7 +1030,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -1024,7 +1048,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>44968</v>
       </c>
@@ -1042,7 +1066,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>44968</v>
       </c>
@@ -1060,7 +1084,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
@@ -1078,7 +1102,7 @@
         <v>6.56</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>45240</v>
       </c>
@@ -1096,7 +1120,7 @@
         <v>77.14</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -1114,7 +1138,7 @@
         <v>4.18</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -1133,6 +1157,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F33" xr:uid="{0F11435F-E248-4A4A-95C5-DA56F5DB2DC5}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="TAC01114990"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
almost there, added test
</commit_message>
<xml_diff>
--- a/data/bdFile.xlsx
+++ b/data/bdFile.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lesleycheung/Desktop/mazen/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97613AF0-5467-A94E-B2BF-5448FAA86464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562952D2-3C1B-1C47-A5C3-E55F32714EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34800" yWindow="-21100" windowWidth="19200" windowHeight="21100" xr2:uid="{F2FF1488-102E-7448-BBB7-46247D1761A1}"/>
+    <workbookView xWindow="34820" yWindow="-21100" windowWidth="19200" windowHeight="21100" xr2:uid="{F2FF1488-102E-7448-BBB7-46247D1761A1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Original" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$A$1:$F$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$F$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="30">
   <si>
     <t>TAC00070840</t>
   </si>
@@ -56,9 +58,6 @@
     <t>TAC11179670</t>
   </si>
   <si>
-    <t>TAC11179680</t>
-  </si>
-  <si>
     <t>TAC11179770</t>
   </si>
   <si>
@@ -117,9 +116,6 @@
   </si>
   <si>
     <t>10/28/23</t>
-  </si>
-  <si>
-    <t>practice</t>
   </si>
   <si>
     <t>09/19/23</t>
@@ -156,7 +152,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,8 +183,20 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -196,31 +204,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -536,12 +571,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F11435F-E248-4A4A-95C5-DA56F5DB2DC5}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:F33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8215AAA-E003-4F47-A936-4C9F93C8BA93}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,32 +586,32 @@
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
-    <col min="6" max="6" width="29.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -590,9 +627,9 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -608,9 +645,9 @@
         <v>15.97</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -626,9 +663,9 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>0</v>
@@ -645,7 +682,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6" s="7">
         <v>45270</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -662,9 +699,9 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>21</v>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
@@ -680,9 +717,9 @@
         <v>6.05</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>22</v>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
@@ -698,49 +735,49 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>22</v>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>1.641</v>
       </c>
       <c r="D9" s="1">
         <v>1.641</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>22</v>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>3.581</v>
       </c>
       <c r="D10" s="1">
         <v>3.581</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
@@ -752,14 +789,14 @@
         <v>1.663</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
         <v>45026</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -772,20 +809,20 @@
         <v>2.4550000000000001</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="5">
+        <v>22</v>
+      </c>
+      <c r="F12" s="4">
         <v>5.84</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
         <v>45026</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>8.2989999999999995</v>
       </c>
       <c r="D13" s="1">
@@ -796,14 +833,14 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
         <v>45148</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>1.6240000000000001</v>
       </c>
       <c r="D14" s="1">
@@ -814,14 +851,14 @@
         <v>1.62</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
         <v>45148</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>1.6240000000000001</v>
       </c>
       <c r="D15" s="1">
@@ -832,14 +869,14 @@
         <v>1.62</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>25</v>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>0.26400000000000001</v>
       </c>
       <c r="D16" s="1">
@@ -850,14 +887,14 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
-        <v>25</v>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>0.26400000000000001</v>
       </c>
       <c r="D17" s="1">
@@ -868,302 +905,573 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>24</v>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="1">
-        <v>1.3480000000000001</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="D18" s="1">
-        <v>1.3480000000000001</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E18" s="1"/>
       <c r="F18" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
-        <v>45026</v>
+        <v>2.4900000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="1">
-        <v>62.356000000000002</v>
+        <v>3.09</v>
       </c>
       <c r="D19" s="1">
-        <v>3.552</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E19" s="1"/>
       <c r="F19" s="1">
-        <v>58.8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
-        <v>45148</v>
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="10">
+        <v>45026</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C20" s="1">
-        <v>12.14</v>
+        <v>37.35</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1">
-        <v>12.14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+        <v>37.35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C21" s="1">
-        <v>71.540000000000006</v>
-      </c>
-      <c r="D21" s="1"/>
+        <v>36.308</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="F21" s="1">
+        <v>36.31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C22" s="1">
-        <v>2.4900000000000002</v>
+        <v>0.11799999999999999</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1">
-        <v>2.4900000000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C23" s="1">
-        <v>3.09</v>
+        <v>0.874</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1">
-        <v>3.09</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
-        <v>45026</v>
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="7">
+        <v>44968</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C24" s="1">
-        <v>37.35</v>
+        <v>0.46300000000000002</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1">
-        <v>37.35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="7">
+        <v>44968</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="1">
-        <v>36.308</v>
+        <v>0.46300000000000002</v>
       </c>
       <c r="D25" s="1">
         <v>0</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1">
-        <v>36.31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>29</v>
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="1">
-        <v>0.11799999999999999</v>
+        <v>6.5620000000000003</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>29</v>
+        <v>6.56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="10">
+        <v>45209</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C27" s="1">
-        <v>0.874</v>
+        <v>77.141000000000005</v>
       </c>
       <c r="D27" s="1">
         <v>0</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
-        <v>44968</v>
+        <v>77.14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C28" s="1">
-        <v>0.46300000000000002</v>
+        <v>4.1779999999999999</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1">
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4">
-        <v>44968</v>
+        <v>4.18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C29" s="1">
-        <v>0.46300000000000002</v>
+        <v>4.4779999999999998</v>
       </c>
       <c r="D29" s="1">
         <v>0</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1">
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" s="1">
-        <v>6.5620000000000003</v>
-      </c>
-      <c r="D30" s="1">
-        <v>0</v>
-      </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1">
-        <v>6.56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="4">
-        <v>45240</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="1">
-        <v>77.141000000000005</v>
-      </c>
-      <c r="D31" s="1">
-        <v>0</v>
-      </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1">
-        <v>77.14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="1" t="s">
+        <v>4.4800000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F29" xr:uid="{0F11435F-E248-4A4A-95C5-DA56F5DB2DC5}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="91" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F11435F-E248-4A4A-95C5-DA56F5DB2DC5}">
+  <sheetPr filterMode="1">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="1">
-        <v>4.1779999999999999</v>
-      </c>
-      <c r="D32" s="1">
-        <v>0</v>
-      </c>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1">
-        <v>4.18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="1">
-        <v>4.4779999999999998</v>
-      </c>
-      <c r="D33" s="1">
-        <v>0</v>
-      </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1">
-        <v>4.4800000000000004</v>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>12.903</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>15.971</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1">
+        <v>15.97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>11.098000000000001</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4.5750000000000002</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1">
+        <v>4.58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>45270</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.878</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6.0460000000000003</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1">
+        <v>6.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2.101</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="9">
+        <v>1.641</v>
+      </c>
+      <c r="D9" s="8">
+        <v>1.641</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="9">
+        <v>3.581</v>
+      </c>
+      <c r="D10" s="8">
+        <v>3.581</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="8">
+        <v>1.663</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1.663</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>45026</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="8">
+        <v>8.2989999999999995</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2.4550000000000001</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="9">
+        <v>5.84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>45026</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="4">
+        <v>8.2989999999999995</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>45148</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1.6240000000000001</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>45148</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1.6240000000000001</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1">
+        <v>0.26</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F33" xr:uid="{0F11435F-E248-4A4A-95C5-DA56F5DB2DC5}">
+  <autoFilter ref="A1:F17" xr:uid="{0F11435F-E248-4A4A-95C5-DA56F5DB2DC5}">
     <filterColumn colId="1">
       <filters>
-        <filter val="TAC01114990"/>
+        <filter val="TAC11179670"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="91" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
starting on afters, befores is good
</commit_message>
<xml_diff>
--- a/data/bdFile.xlsx
+++ b/data/bdFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lesleycheung/Desktop/mazen/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562952D2-3C1B-1C47-A5C3-E55F32714EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21396E41-5D33-4340-8E11-BB795AEB4F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34820" yWindow="-21100" windowWidth="19200" windowHeight="21100" xr2:uid="{F2FF1488-102E-7448-BBB7-46247D1761A1}"/>
   </bookViews>
@@ -137,6 +137,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -223,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -252,12 +255,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,11 +597,12 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="10.83203125" style="17"/>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
@@ -590,7 +610,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -610,7 +630,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -628,7 +648,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -646,7 +666,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -664,7 +684,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -682,8 +702,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
-        <v>45270</v>
+      <c r="A6" s="13">
+        <v>45211</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
@@ -700,7 +720,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="14" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -718,7 +738,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -736,7 +756,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -756,7 +776,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -776,7 +796,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -796,8 +816,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
-        <v>45026</v>
+      <c r="A12" s="15">
+        <v>45203</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>4</v>
@@ -816,8 +836,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
-        <v>45026</v>
+      <c r="A13" s="15">
+        <v>45203</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>4</v>
@@ -834,8 +854,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
-        <v>45148</v>
+      <c r="A14" s="15">
+        <v>45207</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>4</v>
@@ -852,8 +872,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="5">
-        <v>45148</v>
+      <c r="A15" s="15">
+        <v>45207</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
@@ -870,7 +890,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -888,7 +908,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -906,7 +926,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -924,7 +944,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -942,8 +962,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="10">
-        <v>45026</v>
+      <c r="A20" s="14">
+        <v>45203</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -960,7 +980,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -978,7 +998,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="13" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -996,7 +1016,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="13" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1014,8 +1034,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="7">
-        <v>44968</v>
+      <c r="A24" s="13">
+        <v>45232</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>7</v>
@@ -1032,8 +1052,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="7">
-        <v>44968</v>
+      <c r="A25" s="13">
+        <v>45232</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>7</v>
@@ -1050,7 +1070,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1068,7 +1088,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="10">
+      <c r="A27" s="14">
         <v>45209</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1086,7 +1106,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="14" t="s">
         <v>29</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1104,7 +1124,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="14" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="1" t="s">

</xml_diff>

<commit_message>
dates, right now. for now 100 but lets see
</commit_message>
<xml_diff>
--- a/data/bdFile.xlsx
+++ b/data/bdFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lesleycheung/Desktop/mazen/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21396E41-5D33-4340-8E11-BB795AEB4F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05ECE71-2913-9440-A550-F013EE3C1DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34820" yWindow="-21100" windowWidth="19200" windowHeight="21100" xr2:uid="{F2FF1488-102E-7448-BBB7-46247D1761A1}"/>
+    <workbookView xWindow="15620" yWindow="-21100" windowWidth="19200" windowHeight="21100" xr2:uid="{F2FF1488-102E-7448-BBB7-46247D1761A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="2" r:id="rId1"/>
@@ -138,7 +138,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -226,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -252,31 +252,28 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,12 +594,12 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="17"/>
+    <col min="1" max="1" width="10.83203125" style="16"/>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
@@ -610,7 +607,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -630,7 +627,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -648,7 +645,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -666,7 +663,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -684,7 +681,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -702,8 +699,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="13">
-        <v>45211</v>
+      <c r="A6" s="12">
+        <v>45270</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
@@ -720,7 +717,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -738,7 +735,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -756,7 +753,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -776,7 +773,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -796,7 +793,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -816,8 +813,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="15">
-        <v>45203</v>
+      <c r="A12" s="14">
+        <v>45026</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>4</v>
@@ -836,8 +833,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="15">
-        <v>45203</v>
+      <c r="A13" s="14">
+        <v>45026</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>4</v>
@@ -854,8 +851,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="15">
-        <v>45207</v>
+      <c r="A14" s="14">
+        <v>45148</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>4</v>
@@ -872,8 +869,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="15">
-        <v>45207</v>
+      <c r="A15" s="14">
+        <v>45148</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
@@ -890,7 +887,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -908,7 +905,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -926,7 +923,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="13" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -944,7 +941,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="13" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -962,8 +959,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="14">
-        <v>45203</v>
+      <c r="A20" s="13">
+        <v>45026</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -980,7 +977,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="12" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -998,7 +995,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1016,7 +1013,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1034,8 +1031,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="13">
-        <v>45232</v>
+      <c r="A24" s="12">
+        <v>44968</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>7</v>
@@ -1052,8 +1049,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="13">
-        <v>45232</v>
+      <c r="A25" s="12">
+        <v>44968</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>7</v>
@@ -1070,7 +1067,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1088,7 +1085,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="14">
+      <c r="A27" s="13">
         <v>45209</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1106,7 +1103,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="13" t="s">
         <v>29</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1124,7 +1121,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="13" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1320,7 +1317,7 @@
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="1">
         <v>1.641</v>
       </c>
       <c r="D9" s="8">
@@ -1340,7 +1337,7 @@
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="1">
         <v>3.581</v>
       </c>
       <c r="D10" s="8">
@@ -1389,7 +1386,7 @@
       <c r="E12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="1">
         <v>5.84</v>
       </c>
     </row>

</xml_diff>

<commit_message>
need ryan to come back to double check
</commit_message>
<xml_diff>
--- a/data/bdFile.xlsx
+++ b/data/bdFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lesleycheung/Desktop/mazen/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05ECE71-2913-9440-A550-F013EE3C1DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36D8A3E-3142-644D-BCDE-FEC52F37FEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15620" yWindow="-21100" windowWidth="19200" windowHeight="21100" xr2:uid="{F2FF1488-102E-7448-BBB7-46247D1761A1}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="30">
   <si>
     <t>TAC00070840</t>
   </si>
@@ -137,10 +137,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="166" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="167" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -154,8 +155,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,6 +206,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -226,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -274,6 +288,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,7 +613,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -630,17 +649,17 @@
       <c r="A2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="B2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="17">
         <v>12.903</v>
       </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1">
+      <c r="D2" s="17">
+        <v>0</v>
+      </c>
+      <c r="E2" s="18"/>
+      <c r="F2" s="17">
         <v>12.9</v>
       </c>
     </row>
@@ -648,17 +667,17 @@
       <c r="A3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="B3" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="17">
         <v>15.971</v>
       </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1">
+      <c r="D3" s="17">
+        <v>0</v>
+      </c>
+      <c r="E3" s="18"/>
+      <c r="F3" s="17">
         <v>15.97</v>
       </c>
     </row>
@@ -666,17 +685,17 @@
       <c r="A4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="B4" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="17">
         <v>11.098000000000001</v>
       </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1">
+      <c r="D4" s="17">
+        <v>0</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="F4" s="17">
         <v>11.1</v>
       </c>
     </row>
@@ -684,17 +703,17 @@
       <c r="A5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="B5" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="17">
         <v>4.5750000000000002</v>
       </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1">
+      <c r="D5" s="17">
+        <v>0</v>
+      </c>
+      <c r="E5" s="18"/>
+      <c r="F5" s="17">
         <v>4.58</v>
       </c>
     </row>
@@ -702,17 +721,17 @@
       <c r="A6" s="12">
         <v>45270</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="17">
         <v>0.878</v>
       </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1">
+      <c r="D6" s="17">
+        <v>0</v>
+      </c>
+      <c r="E6" s="18"/>
+      <c r="F6" s="17">
         <v>0.88</v>
       </c>
     </row>
@@ -720,17 +739,17 @@
       <c r="A7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="17">
         <v>6.0460000000000003</v>
       </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1">
+      <c r="D7" s="17">
+        <v>0</v>
+      </c>
+      <c r="E7" s="18"/>
+      <c r="F7" s="17">
         <v>6.05</v>
       </c>
     </row>
@@ -738,17 +757,17 @@
       <c r="A8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="17">
         <v>2.101</v>
       </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1">
+      <c r="D8" s="17">
+        <v>0</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="17">
         <v>2.1</v>
       </c>
     </row>
@@ -756,19 +775,19 @@
       <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="4">
+      <c r="B9" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="19">
         <v>1.641</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="17">
         <v>1.641</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="1">
+      <c r="E9" s="20">
+        <v>45190</v>
+      </c>
+      <c r="F9" s="17">
         <v>0</v>
       </c>
     </row>
@@ -776,19 +795,19 @@
       <c r="A10" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="4">
+      <c r="B10" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="19">
         <v>3.581</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="17">
         <v>3.581</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="E10" s="20">
+        <v>45190</v>
+      </c>
+      <c r="F10" s="17">
         <v>0</v>
       </c>
     </row>
@@ -796,19 +815,19 @@
       <c r="A11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="1">
+      <c r="B11" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="17">
         <v>1.663</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="17">
         <v>1.663</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="1">
+      <c r="E11" s="20">
+        <v>45190</v>
+      </c>
+      <c r="F11" s="17">
         <v>0</v>
       </c>
     </row>
@@ -816,19 +835,19 @@
       <c r="A12" s="14">
         <v>45026</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1">
+      <c r="B12" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="17">
         <v>8.2989999999999995</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="17">
         <v>2.4550000000000001</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="4">
+      <c r="E12" s="20">
+        <v>45190</v>
+      </c>
+      <c r="F12" s="19">
         <v>5.84</v>
       </c>
     </row>
@@ -836,17 +855,17 @@
       <c r="A13" s="14">
         <v>45026</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="4">
+      <c r="B13" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="19">
         <v>8.2989999999999995</v>
       </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1">
+      <c r="D13" s="17">
+        <v>0</v>
+      </c>
+      <c r="E13" s="18"/>
+      <c r="F13" s="17">
         <v>8.3000000000000007</v>
       </c>
     </row>
@@ -854,17 +873,17 @@
       <c r="A14" s="14">
         <v>45148</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="4">
+      <c r="B14" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="19">
         <v>1.6240000000000001</v>
       </c>
-      <c r="D14" s="1">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1">
+      <c r="D14" s="17">
+        <v>0</v>
+      </c>
+      <c r="E14" s="18"/>
+      <c r="F14" s="17">
         <v>1.62</v>
       </c>
     </row>
@@ -872,17 +891,17 @@
       <c r="A15" s="14">
         <v>45148</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="4">
+      <c r="B15" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="19">
         <v>1.6240000000000001</v>
       </c>
-      <c r="D15" s="1">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1">
+      <c r="D15" s="17">
+        <v>0</v>
+      </c>
+      <c r="E15" s="18"/>
+      <c r="F15" s="17">
         <v>1.62</v>
       </c>
     </row>
@@ -890,17 +909,17 @@
       <c r="A16" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="6">
+      <c r="B16" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="21">
         <v>0.26400000000000001</v>
       </c>
-      <c r="D16" s="1">
-        <v>0</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1">
+      <c r="D16" s="17">
+        <v>0</v>
+      </c>
+      <c r="E16" s="18"/>
+      <c r="F16" s="17">
         <v>0.26</v>
       </c>
     </row>
@@ -908,17 +927,17 @@
       <c r="A17" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="6">
+      <c r="B17" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="21">
         <v>0.26400000000000001</v>
       </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1">
+      <c r="D17" s="17">
+        <v>0</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="17">
         <v>0.26</v>
       </c>
     </row>
@@ -926,17 +945,17 @@
       <c r="A18" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="17">
         <v>2.4900000000000002</v>
       </c>
-      <c r="D18" s="1">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1">
+      <c r="D18" s="17">
+        <v>0</v>
+      </c>
+      <c r="E18" s="18"/>
+      <c r="F18" s="17">
         <v>2.4900000000000002</v>
       </c>
     </row>
@@ -944,17 +963,17 @@
       <c r="A19" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="17">
         <v>3.09</v>
       </c>
-      <c r="D19" s="1">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1">
+      <c r="D19" s="17">
+        <v>0</v>
+      </c>
+      <c r="E19" s="18"/>
+      <c r="F19" s="17">
         <v>3.09</v>
       </c>
     </row>
@@ -962,17 +981,17 @@
       <c r="A20" s="13">
         <v>45026</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="17">
         <v>37.35</v>
       </c>
-      <c r="D20" s="1">
-        <v>0</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1">
+      <c r="D20" s="17">
+        <v>0</v>
+      </c>
+      <c r="E20" s="18"/>
+      <c r="F20" s="17">
         <v>37.35</v>
       </c>
     </row>
@@ -980,17 +999,17 @@
       <c r="A21" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="17">
         <v>36.308</v>
       </c>
-      <c r="D21" s="1">
-        <v>0</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1">
+      <c r="D21" s="17">
+        <v>0</v>
+      </c>
+      <c r="E21" s="18"/>
+      <c r="F21" s="17">
         <v>36.31</v>
       </c>
     </row>
@@ -998,17 +1017,17 @@
       <c r="A22" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="17">
         <v>0.11799999999999999</v>
       </c>
-      <c r="D22" s="1">
-        <v>0</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1">
+      <c r="D22" s="17">
+        <v>0</v>
+      </c>
+      <c r="E22" s="18"/>
+      <c r="F22" s="17">
         <v>0.12</v>
       </c>
     </row>
@@ -1016,17 +1035,17 @@
       <c r="A23" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="17">
         <v>0.874</v>
       </c>
-      <c r="D23" s="1">
-        <v>0</v>
-      </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1">
+      <c r="D23" s="17">
+        <v>0</v>
+      </c>
+      <c r="E23" s="18"/>
+      <c r="F23" s="17">
         <v>0.87</v>
       </c>
     </row>
@@ -1034,17 +1053,17 @@
       <c r="A24" s="12">
         <v>44968</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="17">
         <v>0.46300000000000002</v>
       </c>
-      <c r="D24" s="1">
-        <v>0</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1">
+      <c r="D24" s="17">
+        <v>0</v>
+      </c>
+      <c r="E24" s="18"/>
+      <c r="F24" s="17">
         <v>0.46</v>
       </c>
     </row>
@@ -1052,17 +1071,17 @@
       <c r="A25" s="12">
         <v>44968</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="17">
         <v>0.46300000000000002</v>
       </c>
-      <c r="D25" s="1">
-        <v>0</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1">
+      <c r="D25" s="17">
+        <v>0</v>
+      </c>
+      <c r="E25" s="18"/>
+      <c r="F25" s="17">
         <v>0.46</v>
       </c>
     </row>
@@ -1070,17 +1089,17 @@
       <c r="A26" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="17">
         <v>6.5620000000000003</v>
       </c>
-      <c r="D26" s="1">
-        <v>0</v>
-      </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1">
+      <c r="D26" s="17">
+        <v>0</v>
+      </c>
+      <c r="E26" s="18"/>
+      <c r="F26" s="17">
         <v>6.56</v>
       </c>
     </row>
@@ -1088,17 +1107,17 @@
       <c r="A27" s="13">
         <v>45209</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="17">
         <v>77.141000000000005</v>
       </c>
-      <c r="D27" s="1">
-        <v>0</v>
-      </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1">
+      <c r="D27" s="17">
+        <v>0</v>
+      </c>
+      <c r="E27" s="18"/>
+      <c r="F27" s="17">
         <v>77.14</v>
       </c>
     </row>
@@ -1106,17 +1125,17 @@
       <c r="A28" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="17">
         <v>4.1779999999999999</v>
       </c>
-      <c r="D28" s="1">
-        <v>0</v>
-      </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1">
+      <c r="D28" s="17">
+        <v>0</v>
+      </c>
+      <c r="E28" s="18"/>
+      <c r="F28" s="17">
         <v>4.18</v>
       </c>
     </row>
@@ -1124,17 +1143,17 @@
       <c r="A29" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="17">
         <v>4.4779999999999998</v>
       </c>
-      <c r="D29" s="1">
-        <v>0</v>
-      </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1">
+      <c r="D29" s="17">
+        <v>0</v>
+      </c>
+      <c r="E29" s="18"/>
+      <c r="F29" s="17">
         <v>4.4800000000000004</v>
       </c>
     </row>

</xml_diff>